<commit_message>
Merged PR 66175: Added TCs [252696, 252699]
Added TCs [252696, 252699]

Related work items: #252696, #252699, #677383
</commit_message>
<xml_diff>
--- a/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/Charts_252697.xlsx
+++ b/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/Charts_252697.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A77DA4-3AEE-4EFA-8361-BD5AB0FA16A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E8CB9B-945C-44EF-ABEB-81AB78239ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,9 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>